<commit_message>
Updated ZAF model - 2025-07-29 12:13
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/vt_vervestacks_ZAF_v1.xlsx
+++ b/VerveStacks_ZAF/vt_vervestacks_ZAF_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C146BB44-C6CB-4712-A3B0-0D9C281A8A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B0A7CFA-E10C-4C54-A99C-06C0799D3657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{4BDBE4C0-F064-4B3E-9052-1E290FD8C332}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{A0A47FEF-62D5-42B1-9DBA-0A3AD1FF68FC}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2820,7 +2820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC83F69D-2528-40F8-ACC4-EC25ADF27B7A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AEC285-2F10-4A56-8478-A18FB11AE5B5}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5745,7 +5745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87355D6-FA2B-4E47-8FAF-8DDA6ED6333A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39212D7-6EC5-4995-9BE8-ED666427378F}">
   <dimension ref="A2:T133"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5827,7 +5827,7 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>9.3024000000000037E-2</v>
+        <v>7.4419200000000033E-2</v>
       </c>
       <c r="E4">
         <v>3583</v>
@@ -5883,7 +5883,7 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>9.3024000000000037E-2</v>
+        <v>7.4419200000000033E-2</v>
       </c>
       <c r="E5">
         <v>3583</v>
@@ -5939,7 +5939,7 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>9.3024000000000037E-2</v>
+        <v>7.4419200000000033E-2</v>
       </c>
       <c r="E6">
         <v>3583</v>
@@ -5995,7 +5995,7 @@
         <v>12</v>
       </c>
       <c r="D7">
-        <v>9.3024000000000037E-2</v>
+        <v>7.4419200000000033E-2</v>
       </c>
       <c r="E7">
         <v>3583</v>
@@ -6051,7 +6051,7 @@
         <v>12</v>
       </c>
       <c r="D8">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E8">
         <v>2445</v>
@@ -6107,7 +6107,7 @@
         <v>12</v>
       </c>
       <c r="D9">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E9">
         <v>2445</v>
@@ -6163,7 +6163,7 @@
         <v>12</v>
       </c>
       <c r="D10">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E10">
         <v>3583</v>
@@ -6219,7 +6219,7 @@
         <v>12</v>
       </c>
       <c r="D11">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E11">
         <v>3583</v>
@@ -6275,7 +6275,7 @@
         <v>12</v>
       </c>
       <c r="D12">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E12">
         <v>3583</v>
@@ -6331,7 +6331,7 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E13">
         <v>3583</v>
@@ -6387,7 +6387,7 @@
         <v>12</v>
       </c>
       <c r="D14">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E14">
         <v>3583</v>
@@ -6443,7 +6443,7 @@
         <v>12</v>
       </c>
       <c r="D15">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E15">
         <v>3583</v>
@@ -6499,7 +6499,7 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E16">
         <v>3583</v>
@@ -6555,7 +6555,7 @@
         <v>12</v>
       </c>
       <c r="D17">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E17">
         <v>3583</v>
@@ -6611,7 +6611,7 @@
         <v>12</v>
       </c>
       <c r="D18">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E18">
         <v>2445</v>
@@ -6667,7 +6667,7 @@
         <v>12</v>
       </c>
       <c r="D19">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E19">
         <v>2445</v>
@@ -6723,19 +6723,19 @@
         <v>12</v>
       </c>
       <c r="D20">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E20">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F20">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G20">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H20">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I20" t="s">
         <v>29</v>
@@ -6779,19 +6779,19 @@
         <v>12</v>
       </c>
       <c r="D21">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E21">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F21">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G21">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H21">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I21" t="s">
         <v>30</v>
@@ -6835,19 +6835,19 @@
         <v>12</v>
       </c>
       <c r="D22">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E22">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F22">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G22">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H22">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I22" t="s">
         <v>31</v>
@@ -6891,19 +6891,19 @@
         <v>12</v>
       </c>
       <c r="D23">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E23">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F23">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G23">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H23">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I23" t="s">
         <v>32</v>
@@ -6947,7 +6947,7 @@
         <v>12</v>
       </c>
       <c r="D24">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E24">
         <v>3583</v>
@@ -7003,7 +7003,7 @@
         <v>12</v>
       </c>
       <c r="D25">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E25">
         <v>3583</v>
@@ -7059,7 +7059,7 @@
         <v>12</v>
       </c>
       <c r="D26">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E26">
         <v>3583</v>
@@ -7115,7 +7115,7 @@
         <v>12</v>
       </c>
       <c r="D27">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E27">
         <v>3583</v>
@@ -7171,7 +7171,7 @@
         <v>12</v>
       </c>
       <c r="D28">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E28">
         <v>3583</v>
@@ -7227,7 +7227,7 @@
         <v>12</v>
       </c>
       <c r="D29">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E29">
         <v>3583</v>
@@ -7283,7 +7283,7 @@
         <v>12</v>
       </c>
       <c r="D30">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E30">
         <v>3583</v>
@@ -7339,7 +7339,7 @@
         <v>12</v>
       </c>
       <c r="D31">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E31">
         <v>3583</v>
@@ -7395,7 +7395,7 @@
         <v>12</v>
       </c>
       <c r="D32">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E32">
         <v>3583</v>
@@ -7451,7 +7451,7 @@
         <v>12</v>
       </c>
       <c r="D33">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E33">
         <v>3583</v>
@@ -7507,7 +7507,7 @@
         <v>12</v>
       </c>
       <c r="D34">
-        <v>8.2080000000000014E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E34">
         <v>3583</v>
@@ -7563,7 +7563,7 @@
         <v>12</v>
       </c>
       <c r="D35">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E35">
         <v>3583</v>
@@ -7619,7 +7619,7 @@
         <v>12</v>
       </c>
       <c r="D36">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E36">
         <v>3583</v>
@@ -7675,7 +7675,7 @@
         <v>12</v>
       </c>
       <c r="D37">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E37">
         <v>3583</v>
@@ -7731,7 +7731,7 @@
         <v>12</v>
       </c>
       <c r="D38">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E38">
         <v>3583</v>
@@ -7787,7 +7787,7 @@
         <v>12</v>
       </c>
       <c r="D39">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000023E-2</v>
       </c>
       <c r="E39">
         <v>3583</v>
@@ -7843,7 +7843,7 @@
         <v>12</v>
       </c>
       <c r="D40">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E40">
         <v>3583</v>
@@ -7899,7 +7899,7 @@
         <v>12</v>
       </c>
       <c r="D41">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E41">
         <v>3583</v>
@@ -7955,7 +7955,7 @@
         <v>12</v>
       </c>
       <c r="D42">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E42">
         <v>3583</v>
@@ -8011,7 +8011,7 @@
         <v>12</v>
       </c>
       <c r="D43">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E43">
         <v>3583</v>
@@ -8067,7 +8067,7 @@
         <v>12</v>
       </c>
       <c r="D44">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E44">
         <v>3583</v>
@@ -8123,7 +8123,7 @@
         <v>12</v>
       </c>
       <c r="D45">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E45">
         <v>3583</v>
@@ -8179,7 +8179,7 @@
         <v>12</v>
       </c>
       <c r="D46">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E46">
         <v>3583</v>
@@ -8235,19 +8235,19 @@
         <v>12</v>
       </c>
       <c r="D47">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E47">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F47">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G47">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H47">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I47" t="s">
         <v>56</v>
@@ -8291,19 +8291,19 @@
         <v>12</v>
       </c>
       <c r="D48">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E48">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F48">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G48">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H48">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I48" t="s">
         <v>57</v>
@@ -8347,19 +8347,19 @@
         <v>12</v>
       </c>
       <c r="D49">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E49">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F49">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G49">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H49">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I49" t="s">
         <v>58</v>
@@ -8403,19 +8403,19 @@
         <v>12</v>
       </c>
       <c r="D50">
-        <v>0.23652000000000001</v>
+        <v>0.17988480000000004</v>
       </c>
       <c r="E50">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F50">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G50">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H50">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I50" t="s">
         <v>59</v>
@@ -8459,19 +8459,19 @@
         <v>12</v>
       </c>
       <c r="D51">
-        <v>0.23652000000000001</v>
+        <v>0.17988480000000004</v>
       </c>
       <c r="E51">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F51">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G51">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H51">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I51" t="s">
         <v>60</v>
@@ -8515,19 +8515,19 @@
         <v>12</v>
       </c>
       <c r="D52">
-        <v>0.23652000000000001</v>
+        <v>0.17988480000000004</v>
       </c>
       <c r="E52">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F52">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G52">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H52">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I52" t="s">
         <v>61</v>
@@ -8571,7 +8571,7 @@
         <v>12</v>
       </c>
       <c r="D53">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E53">
         <v>2445</v>
@@ -8627,7 +8627,7 @@
         <v>12</v>
       </c>
       <c r="D54">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E54">
         <v>2445</v>
@@ -8683,7 +8683,7 @@
         <v>12</v>
       </c>
       <c r="D55">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E55">
         <v>2445</v>
@@ -8739,7 +8739,7 @@
         <v>12</v>
       </c>
       <c r="D56">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E56">
         <v>2445</v>
@@ -8795,7 +8795,7 @@
         <v>12</v>
       </c>
       <c r="D57">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E57">
         <v>2445</v>
@@ -8851,7 +8851,7 @@
         <v>12</v>
       </c>
       <c r="D58">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E58">
         <v>2445</v>
@@ -8907,19 +8907,19 @@
         <v>12</v>
       </c>
       <c r="D59">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E59">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F59">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G59">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H59">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I59" t="s">
         <v>68</v>
@@ -8963,19 +8963,19 @@
         <v>12</v>
       </c>
       <c r="D60">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E60">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F60">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G60">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H60">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I60" t="s">
         <v>69</v>
@@ -9019,19 +9019,19 @@
         <v>12</v>
       </c>
       <c r="D61">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E61">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F61">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G61">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H61">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I61" t="s">
         <v>70</v>
@@ -9075,19 +9075,19 @@
         <v>12</v>
       </c>
       <c r="D62">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E62">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F62">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G62">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H62">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I62" t="s">
         <v>71</v>
@@ -9131,19 +9131,19 @@
         <v>12</v>
       </c>
       <c r="D63">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E63">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F63">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G63">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H63">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I63" t="s">
         <v>72</v>
@@ -9187,19 +9187,19 @@
         <v>12</v>
       </c>
       <c r="D64">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E64">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F64">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G64">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H64">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I64" t="s">
         <v>73</v>
@@ -9243,19 +9243,19 @@
         <v>12</v>
       </c>
       <c r="D65">
-        <v>0.23652000000000001</v>
+        <v>0.17988480000000004</v>
       </c>
       <c r="E65">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F65">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G65">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H65">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I65" t="s">
         <v>74</v>
@@ -9299,19 +9299,19 @@
         <v>12</v>
       </c>
       <c r="D66">
-        <v>0.23652000000000001</v>
+        <v>0.17988480000000004</v>
       </c>
       <c r="E66">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F66">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G66">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H66">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I66" t="s">
         <v>75</v>
@@ -9355,19 +9355,19 @@
         <v>12</v>
       </c>
       <c r="D67">
-        <v>0.23652000000000001</v>
+        <v>0.17988480000000004</v>
       </c>
       <c r="E67">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F67">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G67">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H67">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I67" t="s">
         <v>76</v>
@@ -9411,19 +9411,19 @@
         <v>12</v>
       </c>
       <c r="D68">
-        <v>0.26729999999999998</v>
+        <v>0.20839680000000005</v>
       </c>
       <c r="E68">
-        <v>1923</v>
+        <v>2126</v>
       </c>
       <c r="F68">
-        <v>22.9</v>
+        <v>25.1</v>
       </c>
       <c r="G68">
-        <v>2.88</v>
+        <v>3.22</v>
       </c>
       <c r="H68">
-        <v>0.80844999999999989</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I68" t="s">
         <v>77</v>
@@ -9467,19 +9467,19 @@
         <v>12</v>
       </c>
       <c r="D69">
-        <v>0.26729999999999998</v>
+        <v>0.20839680000000005</v>
       </c>
       <c r="E69">
-        <v>1923</v>
+        <v>2126</v>
       </c>
       <c r="F69">
-        <v>22.9</v>
+        <v>25.1</v>
       </c>
       <c r="G69">
-        <v>2.88</v>
+        <v>3.22</v>
       </c>
       <c r="H69">
-        <v>0.80844999999999989</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I69" t="s">
         <v>78</v>
@@ -9523,19 +9523,19 @@
         <v>12</v>
       </c>
       <c r="D70">
-        <v>0.26729999999999998</v>
+        <v>0.20839680000000005</v>
       </c>
       <c r="E70">
-        <v>1923</v>
+        <v>2126</v>
       </c>
       <c r="F70">
-        <v>22.9</v>
+        <v>25.1</v>
       </c>
       <c r="G70">
-        <v>2.88</v>
+        <v>3.22</v>
       </c>
       <c r="H70">
-        <v>0.80844999999999989</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I70" t="s">
         <v>79</v>
@@ -9579,19 +9579,19 @@
         <v>12</v>
       </c>
       <c r="D71">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E71">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F71">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G71">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H71">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I71" t="s">
         <v>80</v>
@@ -9635,19 +9635,19 @@
         <v>12</v>
       </c>
       <c r="D72">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E72">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F72">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G72">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H72">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I72" t="s">
         <v>81</v>
@@ -9691,19 +9691,19 @@
         <v>12</v>
       </c>
       <c r="D73">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E73">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F73">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G73">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H73">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I73" t="s">
         <v>82</v>
@@ -9747,19 +9747,19 @@
         <v>12</v>
       </c>
       <c r="D74">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E74">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F74">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G74">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H74">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I74" t="s">
         <v>83</v>
@@ -9803,19 +9803,19 @@
         <v>12</v>
       </c>
       <c r="D75">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E75">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F75">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G75">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H75">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I75" t="s">
         <v>84</v>
@@ -9859,19 +9859,19 @@
         <v>12</v>
       </c>
       <c r="D76">
-        <v>0.23652000000000001</v>
+        <v>0.17988480000000004</v>
       </c>
       <c r="E76">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F76">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G76">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H76">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I76" t="s">
         <v>85</v>
@@ -9915,7 +9915,7 @@
         <v>12</v>
       </c>
       <c r="D77">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E77">
         <v>2445</v>
@@ -9971,7 +9971,7 @@
         <v>12</v>
       </c>
       <c r="D78">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E78">
         <v>2445</v>
@@ -10027,7 +10027,7 @@
         <v>12</v>
       </c>
       <c r="D79">
-        <v>0.21236400000000008</v>
+        <v>0.16989120000000002</v>
       </c>
       <c r="E79">
         <v>2445</v>
@@ -10083,19 +10083,19 @@
         <v>12</v>
       </c>
       <c r="D80">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E80">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F80">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G80">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H80">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I80" t="s">
         <v>89</v>
@@ -10139,19 +10139,19 @@
         <v>12</v>
       </c>
       <c r="D81">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E81">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F81">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G81">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H81">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I81" t="s">
         <v>90</v>
@@ -10195,19 +10195,19 @@
         <v>12</v>
       </c>
       <c r="D82">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E82">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F82">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G82">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H82">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I82" t="s">
         <v>91</v>
@@ -10251,7 +10251,7 @@
         <v>12</v>
       </c>
       <c r="D83">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E83">
         <v>3583</v>
@@ -10307,7 +10307,7 @@
         <v>12</v>
       </c>
       <c r="D84">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E84">
         <v>3583</v>
@@ -10363,7 +10363,7 @@
         <v>12</v>
       </c>
       <c r="D85">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E85">
         <v>3583</v>
@@ -10419,7 +10419,7 @@
         <v>12</v>
       </c>
       <c r="D86">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E86">
         <v>3583</v>
@@ -10475,7 +10475,7 @@
         <v>12</v>
       </c>
       <c r="D87">
-        <v>8.2080000000000042E-2</v>
+        <v>6.5664000000000014E-2</v>
       </c>
       <c r="E87">
         <v>3583</v>
@@ -10531,19 +10531,19 @@
         <v>12</v>
       </c>
       <c r="D88">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E88">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F88">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G88">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H88">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I88" t="s">
         <v>97</v>
@@ -10587,19 +10587,19 @@
         <v>12</v>
       </c>
       <c r="D89">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E89">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F89">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G89">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H89">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I89" t="s">
         <v>98</v>
@@ -10643,19 +10643,19 @@
         <v>12</v>
       </c>
       <c r="D90">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E90">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F90">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G90">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H90">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I90" t="s">
         <v>99</v>
@@ -10699,19 +10699,19 @@
         <v>12</v>
       </c>
       <c r="D91">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E91">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F91">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G91">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H91">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I91" t="s">
         <v>100</v>
@@ -10755,19 +10755,19 @@
         <v>12</v>
       </c>
       <c r="D92">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E92">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F92">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G92">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H92">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I92" t="s">
         <v>101</v>
@@ -10811,19 +10811,19 @@
         <v>12</v>
       </c>
       <c r="D93">
-        <v>0.22995000000000002</v>
+        <v>0.17488800000000002</v>
       </c>
       <c r="E93">
-        <v>2200</v>
+        <v>2445</v>
       </c>
       <c r="F93">
-        <v>27.7</v>
+        <v>30.4</v>
       </c>
       <c r="G93">
-        <v>3.1</v>
+        <v>3.52</v>
       </c>
       <c r="H93">
-        <v>0.74765000000000004</v>
+        <v>0.72770000000000001</v>
       </c>
       <c r="I93" t="s">
         <v>102</v>
@@ -10867,7 +10867,7 @@
         <v>12</v>
       </c>
       <c r="D94">
-        <v>7.3872000000000021E-2</v>
+        <v>5.9097600000000014E-2</v>
       </c>
       <c r="E94">
         <v>3583</v>
@@ -10923,7 +10923,7 @@
         <v>12</v>
       </c>
       <c r="D95">
-        <v>8.7552000000000019E-2</v>
+        <v>7.0041600000000037E-2</v>
       </c>
       <c r="E95">
         <v>3583</v>
@@ -10979,19 +10979,19 @@
         <v>12</v>
       </c>
       <c r="D96">
-        <v>0.31560749999999999</v>
+        <v>0.24023520000000001</v>
       </c>
       <c r="E96">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F96">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G96">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H96">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I96" t="s">
         <v>104</v>
@@ -11035,19 +11035,19 @@
         <v>12</v>
       </c>
       <c r="D97">
-        <v>0.31560749999999999</v>
+        <v>0.24023520000000001</v>
       </c>
       <c r="E97">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F97">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G97">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H97">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I97" t="s">
         <v>105</v>
@@ -11091,19 +11091,19 @@
         <v>12</v>
       </c>
       <c r="D98">
-        <v>0.32321250000000001</v>
+        <v>0.24602400000000008</v>
       </c>
       <c r="E98">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F98">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G98">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H98">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I98" t="s">
         <v>106</v>
@@ -11147,19 +11147,19 @@
         <v>12</v>
       </c>
       <c r="D99">
-        <v>0.32321250000000001</v>
+        <v>0.24602400000000008</v>
       </c>
       <c r="E99">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F99">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G99">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H99">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I99" t="s">
         <v>107</v>
@@ -11203,19 +11203,19 @@
         <v>12</v>
       </c>
       <c r="D100">
-        <v>0.32321250000000001</v>
+        <v>0.24602400000000008</v>
       </c>
       <c r="E100">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F100">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G100">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H100">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I100" t="s">
         <v>108</v>
@@ -11259,19 +11259,19 @@
         <v>12</v>
       </c>
       <c r="D101">
-        <v>0.32321250000000001</v>
+        <v>0.24602400000000008</v>
       </c>
       <c r="E101">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F101">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G101">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H101">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I101" t="s">
         <v>109</v>
@@ -11315,19 +11315,19 @@
         <v>12</v>
       </c>
       <c r="D102">
-        <v>0.32321250000000001</v>
+        <v>0.24602400000000008</v>
       </c>
       <c r="E102">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F102">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G102">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H102">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I102" t="s">
         <v>110</v>
@@ -11371,19 +11371,19 @@
         <v>12</v>
       </c>
       <c r="D103">
-        <v>0.31560749999999999</v>
+        <v>0.24023520000000001</v>
       </c>
       <c r="E103">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F103">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G103">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H103">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I103" t="s">
         <v>111</v>
@@ -11427,19 +11427,19 @@
         <v>12</v>
       </c>
       <c r="D104">
-        <v>0.31560749999999999</v>
+        <v>0.24023520000000001</v>
       </c>
       <c r="E104">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F104">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G104">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H104">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I104" t="s">
         <v>112</v>
@@ -11483,19 +11483,19 @@
         <v>12</v>
       </c>
       <c r="D105">
-        <v>0.31560749999999999</v>
+        <v>0.24023520000000001</v>
       </c>
       <c r="E105">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F105">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G105">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H105">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I105" t="s">
         <v>113</v>
@@ -11539,19 +11539,19 @@
         <v>12</v>
       </c>
       <c r="D106">
-        <v>0.31560749999999999</v>
+        <v>0.24023520000000001</v>
       </c>
       <c r="E106">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F106">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G106">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H106">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I106" t="s">
         <v>114</v>
@@ -11595,19 +11595,19 @@
         <v>12</v>
       </c>
       <c r="D107">
-        <v>0.31560749999999999</v>
+        <v>0.24023520000000001</v>
       </c>
       <c r="E107">
-        <v>1726</v>
+        <v>2126</v>
       </c>
       <c r="F107">
-        <v>20.9</v>
+        <v>25.1</v>
       </c>
       <c r="G107">
-        <v>2.5499999999999998</v>
+        <v>3.22</v>
       </c>
       <c r="H107">
-        <v>0.82269999999999999</v>
+        <v>0.79419999999999991</v>
       </c>
       <c r="I107" t="s">
         <v>115</v>
@@ -13102,7 +13102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D09DFC-0B05-4536-B3DF-36B053AECD22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CBF3FDA-E930-4C1B-950A-D5C46BDFABF9}">
   <dimension ref="A2:S263"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13187,7 +13187,7 @@
         <v>7.2300000000000003E-2</v>
       </c>
       <c r="F4">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000008</v>
       </c>
       <c r="G4">
         <v>2295</v>
@@ -13240,7 +13240,7 @@
         <v>0.37</v>
       </c>
       <c r="F5">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G5">
         <v>1700</v>
@@ -13293,7 +13293,7 @@
         <v>0.39</v>
       </c>
       <c r="F6">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G6">
         <v>1700</v>
@@ -13346,7 +13346,7 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="F7">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000007</v>
       </c>
       <c r="G7">
         <v>1700</v>
@@ -13399,7 +13399,7 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="F8">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000007</v>
       </c>
       <c r="G8">
         <v>1700</v>
@@ -13452,7 +13452,7 @@
         <v>0.4</v>
       </c>
       <c r="F9">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G9">
         <v>1700</v>
@@ -13505,7 +13505,7 @@
         <v>0.4</v>
       </c>
       <c r="F10">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G10">
         <v>1700</v>
@@ -13558,7 +13558,7 @@
         <v>0.2</v>
       </c>
       <c r="F11">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G11">
         <v>1955</v>
@@ -13611,7 +13611,7 @@
         <v>0.2</v>
       </c>
       <c r="F12">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G12">
         <v>1955</v>
@@ -13664,7 +13664,7 @@
         <v>0.2</v>
       </c>
       <c r="F13">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G13">
         <v>1955</v>
@@ -13717,7 +13717,7 @@
         <v>0.2</v>
       </c>
       <c r="F14">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G14">
         <v>1955</v>
@@ -13770,7 +13770,7 @@
         <v>0.2</v>
       </c>
       <c r="F15">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G15">
         <v>1955</v>
@@ -13823,7 +13823,7 @@
         <v>0.2</v>
       </c>
       <c r="F16">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G16">
         <v>1955</v>
@@ -13876,7 +13876,7 @@
         <v>0.2</v>
       </c>
       <c r="F17">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G17">
         <v>1955</v>
@@ -13929,7 +13929,7 @@
         <v>0.2</v>
       </c>
       <c r="F18">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G18">
         <v>1955</v>
@@ -13982,7 +13982,7 @@
         <v>0.6</v>
       </c>
       <c r="F19">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G19">
         <v>1700</v>
@@ -14035,7 +14035,7 @@
         <v>0.6</v>
       </c>
       <c r="F20">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G20">
         <v>1700</v>
@@ -14088,7 +14088,7 @@
         <v>0.6</v>
       </c>
       <c r="F21">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G21">
         <v>1700</v>
@@ -14141,7 +14141,7 @@
         <v>0.6</v>
       </c>
       <c r="F22">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G22">
         <v>1700</v>
@@ -14194,7 +14194,7 @@
         <v>0.6</v>
       </c>
       <c r="F23">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G23">
         <v>1700</v>
@@ -14247,7 +14247,7 @@
         <v>0.6</v>
       </c>
       <c r="F24">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G24">
         <v>1700</v>
@@ -14300,7 +14300,7 @@
         <v>0.2</v>
       </c>
       <c r="F25">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G25">
         <v>1955</v>
@@ -14353,7 +14353,7 @@
         <v>0.2</v>
       </c>
       <c r="F26">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G26">
         <v>1955</v>
@@ -14406,7 +14406,7 @@
         <v>0.2</v>
       </c>
       <c r="F27">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G27">
         <v>1955</v>
@@ -14459,7 +14459,7 @@
         <v>0.2</v>
       </c>
       <c r="F28">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G28">
         <v>1955</v>
@@ -14512,7 +14512,7 @@
         <v>0.19</v>
       </c>
       <c r="F29">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G29">
         <v>1955</v>
@@ -14565,7 +14565,7 @@
         <v>0.2</v>
       </c>
       <c r="F30">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G30">
         <v>1955</v>
@@ -14618,7 +14618,7 @@
         <v>0.2</v>
       </c>
       <c r="F31">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G31">
         <v>1955</v>
@@ -14671,7 +14671,7 @@
         <v>0.2</v>
       </c>
       <c r="F32">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G32">
         <v>1955</v>
@@ -14724,7 +14724,7 @@
         <v>0.2</v>
       </c>
       <c r="F33">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G33">
         <v>1955</v>
@@ -14777,7 +14777,7 @@
         <v>0.2</v>
       </c>
       <c r="F34">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G34">
         <v>1955</v>
@@ -14830,7 +14830,7 @@
         <v>0.2</v>
       </c>
       <c r="F35">
-        <v>0.27</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G35">
         <v>1955</v>
@@ -14883,7 +14883,7 @@
         <v>0.2</v>
       </c>
       <c r="F36">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G36">
         <v>1955</v>
@@ -14936,7 +14936,7 @@
         <v>0.2</v>
       </c>
       <c r="F37">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G37">
         <v>1955</v>
@@ -14989,7 +14989,7 @@
         <v>0.2</v>
       </c>
       <c r="F38">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G38">
         <v>1955</v>
@@ -15042,7 +15042,7 @@
         <v>0.2</v>
       </c>
       <c r="F39">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G39">
         <v>1955</v>
@@ -15095,7 +15095,7 @@
         <v>0.2</v>
       </c>
       <c r="F40">
-        <v>0.28800000000000003</v>
+        <v>0.23040000000000005</v>
       </c>
       <c r="G40">
         <v>1955</v>
@@ -15148,7 +15148,7 @@
         <v>0.06</v>
       </c>
       <c r="F41">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G41">
         <v>1955</v>
@@ -15201,7 +15201,7 @@
         <v>0.06</v>
       </c>
       <c r="F42">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G42">
         <v>1955</v>
@@ -15254,7 +15254,7 @@
         <v>0.06</v>
       </c>
       <c r="F43">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G43">
         <v>1955</v>
@@ -15307,7 +15307,7 @@
         <v>0.06</v>
       </c>
       <c r="F44">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G44">
         <v>1955</v>
@@ -15360,7 +15360,7 @@
         <v>0.06</v>
       </c>
       <c r="F45">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G45">
         <v>1955</v>
@@ -15413,7 +15413,7 @@
         <v>0.06</v>
       </c>
       <c r="F46">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G46">
         <v>1955</v>
@@ -15466,7 +15466,7 @@
         <v>0.06</v>
       </c>
       <c r="F47">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G47">
         <v>1955</v>
@@ -15519,7 +15519,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="F48">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G48">
         <v>1700</v>
@@ -15572,7 +15572,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="F49">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G49">
         <v>1700</v>
@@ -15625,7 +15625,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="F50">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G50">
         <v>1700</v>
@@ -15678,7 +15678,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="F51">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G51">
         <v>1700</v>
@@ -15731,7 +15731,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="F52">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G52">
         <v>1700</v>
@@ -15784,7 +15784,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="F53">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G53">
         <v>1700</v>
@@ -15837,7 +15837,7 @@
         <v>0.5</v>
       </c>
       <c r="F54">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G54">
         <v>1700</v>
@@ -15890,7 +15890,7 @@
         <v>0.5</v>
       </c>
       <c r="F55">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G55">
         <v>1700</v>
@@ -15943,7 +15943,7 @@
         <v>0.5</v>
       </c>
       <c r="F56">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G56">
         <v>1700</v>
@@ -15996,7 +15996,7 @@
         <v>0.5</v>
       </c>
       <c r="F57">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G57">
         <v>1700</v>
@@ -16049,7 +16049,7 @@
         <v>0.5</v>
       </c>
       <c r="F58">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G58">
         <v>1700</v>
@@ -16102,7 +16102,7 @@
         <v>0.5</v>
       </c>
       <c r="F59">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G59">
         <v>1700</v>
@@ -16155,7 +16155,7 @@
         <v>0.61799999999999999</v>
       </c>
       <c r="F60">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G60">
         <v>1700</v>
@@ -16208,7 +16208,7 @@
         <v>0.61799999999999999</v>
       </c>
       <c r="F61">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G61">
         <v>1700</v>
@@ -16261,7 +16261,7 @@
         <v>0.61799999999999999</v>
       </c>
       <c r="F62">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G62">
         <v>1700</v>
@@ -16314,7 +16314,7 @@
         <v>0.61799999999999999</v>
       </c>
       <c r="F63">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G63">
         <v>1700</v>
@@ -16367,7 +16367,7 @@
         <v>0.61799999999999999</v>
       </c>
       <c r="F64">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G64">
         <v>1700</v>
@@ -16420,7 +16420,7 @@
         <v>0.61799999999999999</v>
       </c>
       <c r="F65">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G65">
         <v>1700</v>
@@ -16473,7 +16473,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F66">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G66">
         <v>1700</v>
@@ -16526,7 +16526,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F67">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G67">
         <v>1700</v>
@@ -16579,7 +16579,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F68">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G68">
         <v>1700</v>
@@ -16632,7 +16632,7 @@
         <v>0.71599999999999997</v>
       </c>
       <c r="F69">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G69">
         <v>1700</v>
@@ -16685,7 +16685,7 @@
         <v>0.71599999999999997</v>
       </c>
       <c r="F70">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G70">
         <v>1700</v>
@@ -16738,7 +16738,7 @@
         <v>0.71599999999999997</v>
       </c>
       <c r="F71">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G71">
         <v>1700</v>
@@ -16791,7 +16791,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F72">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G72">
         <v>1700</v>
@@ -16844,7 +16844,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F73">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G73">
         <v>1700</v>
@@ -16897,7 +16897,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F74">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G74">
         <v>1700</v>
@@ -16950,7 +16950,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F75">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G75">
         <v>1700</v>
@@ -17003,7 +17003,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F76">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G76">
         <v>1700</v>
@@ -17056,7 +17056,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F77">
-        <v>0.32400000000000001</v>
+        <v>0.25920000000000004</v>
       </c>
       <c r="G77">
         <v>1700</v>
@@ -17109,7 +17109,7 @@
         <v>0.6</v>
       </c>
       <c r="F78">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G78">
         <v>1700</v>
@@ -17162,7 +17162,7 @@
         <v>0.6</v>
       </c>
       <c r="F79">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G79">
         <v>1700</v>
@@ -17215,7 +17215,7 @@
         <v>0.6</v>
       </c>
       <c r="F80">
-        <v>0.30600000000000005</v>
+        <v>0.24480000000000005</v>
       </c>
       <c r="G80">
         <v>1700</v>
@@ -17268,7 +17268,7 @@
         <v>0.6</v>
       </c>
       <c r="F81">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G81">
         <v>1700</v>
@@ -17321,7 +17321,7 @@
         <v>0.6</v>
       </c>
       <c r="F82">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G82">
         <v>1700</v>
@@ -17374,7 +17374,7 @@
         <v>0.6</v>
       </c>
       <c r="F83">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G83">
         <v>1700</v>
@@ -17427,7 +17427,7 @@
         <v>0.06</v>
       </c>
       <c r="F84">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G84">
         <v>1955</v>
@@ -17480,7 +17480,7 @@
         <v>0.06</v>
       </c>
       <c r="F85">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G85">
         <v>1955</v>
@@ -17533,7 +17533,7 @@
         <v>0.06</v>
       </c>
       <c r="F86">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G86">
         <v>1955</v>
@@ -17586,7 +17586,7 @@
         <v>0.06</v>
       </c>
       <c r="F87">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G87">
         <v>1955</v>
@@ -17639,7 +17639,7 @@
         <v>0.06</v>
       </c>
       <c r="F88">
-        <v>0.27000000000000007</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="G88">
         <v>1955</v>
@@ -17692,7 +17692,7 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="F89">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G89">
         <v>1700</v>
@@ -17745,7 +17745,7 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="F90">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G90">
         <v>1700</v>
@@ -17798,7 +17798,7 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="F91">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G91">
         <v>1700</v>
@@ -17851,7 +17851,7 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="F92">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G92">
         <v>1700</v>
@@ -17904,7 +17904,7 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="F93">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G93">
         <v>1700</v>
@@ -17957,7 +17957,7 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="F94">
-        <v>0.315</v>
+        <v>0.252</v>
       </c>
       <c r="G94">
         <v>1700</v>
@@ -18010,7 +18010,7 @@
         <v>0.18</v>
       </c>
       <c r="F95">
-        <v>0.24300000000000002</v>
+        <v>0.19440000000000002</v>
       </c>
       <c r="G95">
         <v>2295</v>
@@ -18063,7 +18063,7 @@
         <v>0.8</v>
       </c>
       <c r="F96">
-        <v>0.3735</v>
+        <v>0.29880000000000001</v>
       </c>
       <c r="G96">
         <v>1870</v>
@@ -18116,7 +18116,7 @@
         <v>0.8</v>
       </c>
       <c r="F97">
-        <v>0.3735</v>
+        <v>0.29880000000000001</v>
       </c>
       <c r="G97">
         <v>1870</v>
@@ -18169,7 +18169,7 @@
         <v>0.8</v>
       </c>
       <c r="F98">
-        <v>0.38250000000000001</v>
+        <v>0.30600000000000005</v>
       </c>
       <c r="G98">
         <v>1870</v>
@@ -18222,7 +18222,7 @@
         <v>0.8</v>
       </c>
       <c r="F99">
-        <v>0.38250000000000001</v>
+        <v>0.30600000000000005</v>
       </c>
       <c r="G99">
         <v>1870</v>
@@ -18275,7 +18275,7 @@
         <v>0.8</v>
       </c>
       <c r="F100">
-        <v>0.38250000000000001</v>
+        <v>0.30600000000000005</v>
       </c>
       <c r="G100">
         <v>1870</v>
@@ -18328,7 +18328,7 @@
         <v>0.8</v>
       </c>
       <c r="F101">
-        <v>0.38250000000000001</v>
+        <v>0.30600000000000005</v>
       </c>
       <c r="G101">
         <v>1870</v>
@@ -18381,7 +18381,7 @@
         <v>0.79479999999999995</v>
       </c>
       <c r="F102">
-        <v>0.38250000000000001</v>
+        <v>0.30600000000000005</v>
       </c>
       <c r="G102">
         <v>1870</v>
@@ -18434,7 +18434,7 @@
         <v>0.79479999999999995</v>
       </c>
       <c r="F103">
-        <v>0.3735</v>
+        <v>0.29880000000000001</v>
       </c>
       <c r="G103">
         <v>1870</v>
@@ -18487,7 +18487,7 @@
         <v>0.79479999999999995</v>
       </c>
       <c r="F104">
-        <v>0.3735</v>
+        <v>0.29880000000000001</v>
       </c>
       <c r="G104">
         <v>1870</v>
@@ -18540,7 +18540,7 @@
         <v>0.79479999999999995</v>
       </c>
       <c r="F105">
-        <v>0.3735</v>
+        <v>0.29880000000000001</v>
       </c>
       <c r="G105">
         <v>1870</v>
@@ -18593,7 +18593,7 @@
         <v>0.79479999999999995</v>
       </c>
       <c r="F106">
-        <v>0.3735</v>
+        <v>0.29880000000000001</v>
       </c>
       <c r="G106">
         <v>1870</v>
@@ -18646,7 +18646,7 @@
         <v>0.79479999999999995</v>
       </c>
       <c r="F107">
-        <v>0.3735</v>
+        <v>0.29880000000000001</v>
       </c>
       <c r="G107">
         <v>1870</v>

</xml_diff>

<commit_message>
Updated ZAF model - 2025-07-29 14:31
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/vt_vervestacks_ZAF_v1.xlsx
+++ b/VerveStacks_ZAF/vt_vervestacks_ZAF_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED7AEFB7-C10C-41FA-A4F8-AF60D960D1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB5CC62E-C882-4A38-B931-67D4F7A0B671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{90E4DB8B-9C9B-40F7-9886-1FA672E1E149}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{146CDEF4-B9C4-4AB0-ABA9-7030D5C733BB}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2820,7 +2820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B9C44C-3B99-4FBE-B2AB-840417904DCB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0130C3B9-63EF-4AD3-901A-5F9614A9B112}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5745,7 +5745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D74917-F3E0-4E45-9C6F-B443C62309BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC37542-4C1A-4F2D-8C7C-DDAAF883EC4F}">
   <dimension ref="A2:T133"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13102,7 +13102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60DAB2D-839D-47DB-A034-D81A0AD726FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC17F27-5182-457F-868E-AA691D4AEF19}">
   <dimension ref="A2:S263"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ZAF model - 2025-07-29 14:33
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/vt_vervestacks_ZAF_v1.xlsx
+++ b/VerveStacks_ZAF/vt_vervestacks_ZAF_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB5CC62E-C882-4A38-B931-67D4F7A0B671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94E2A440-983F-4C5C-A6A7-F610D009F9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{146CDEF4-B9C4-4AB0-ABA9-7030D5C733BB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{9C1171B4-3AAD-451E-9C38-B3A3EC8D10B0}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2820,7 +2820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0130C3B9-63EF-4AD3-901A-5F9614A9B112}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6534C7FC-D34D-4C3E-9982-9ACBC6DCB962}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5745,7 +5745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC37542-4C1A-4F2D-8C7C-DDAAF883EC4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C0667E-2431-48ED-8A59-626555504E40}">
   <dimension ref="A2:T133"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13102,7 +13102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC17F27-5182-457F-868E-AA691D4AEF19}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CEFE27-B42B-419F-B66B-0D1D19ABC34A}">
   <dimension ref="A2:S263"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ZAF model - 2025-07-29 14:41
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/vt_vervestacks_ZAF_v1.xlsx
+++ b/VerveStacks_ZAF/vt_vervestacks_ZAF_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94E2A440-983F-4C5C-A6A7-F610D009F9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50198939-B764-4F45-AAA8-6FC8100177DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{9C1171B4-3AAD-451E-9C38-B3A3EC8D10B0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{FB2BEA45-1298-479D-811B-1F5303290AE9}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2820,7 +2820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6534C7FC-D34D-4C3E-9982-9ACBC6DCB962}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766592E6-9DD1-45B3-A2A6-67F0BF4A007C}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5745,7 +5745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C0667E-2431-48ED-8A59-626555504E40}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F9B694-5E39-4AAF-A3B3-2780567B3CFD}">
   <dimension ref="A2:T133"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13102,7 +13102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CEFE27-B42B-419F-B66B-0D1D19ABC34A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2198CEE1-1274-4D64-8705-BE4F3A0718AE}">
   <dimension ref="A2:S263"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>